<commit_message>
Latest data: Thu Dec  1 04:22:09 UTC 2022
</commit_message>
<xml_diff>
--- a/data/incidenti_pedone.xlsx
+++ b/data/incidenti_pedone.xlsx
@@ -14168,7 +14168,7 @@
         <v>11.35771849964447</v>
       </c>
       <c r="AB104" t="n">
-        <v>46.49680059440739</v>
+        <v>46.4968005944074</v>
       </c>
     </row>
     <row r="105">
@@ -18392,7 +18392,7 @@
         <v>11.35754642734926</v>
       </c>
       <c r="AB136" t="n">
-        <v>46.4974822013345</v>
+        <v>46.49748220133451</v>
       </c>
     </row>
     <row r="137">
@@ -20768,7 +20768,7 @@
         <v>11.32700777610736</v>
       </c>
       <c r="AB154" t="n">
-        <v>46.49279886738609</v>
+        <v>46.4927988673861</v>
       </c>
     </row>
     <row r="155">
@@ -20900,7 +20900,7 @@
         <v>11.34105868970266</v>
       </c>
       <c r="AB155" t="n">
-        <v>46.49292820833486</v>
+        <v>46.49292820833485</v>
       </c>
     </row>
     <row r="156">
@@ -23672,7 +23672,7 @@
         <v>11.33254508264234</v>
       </c>
       <c r="AB176" t="n">
-        <v>46.49584821081341</v>
+        <v>46.49584821081342</v>
       </c>
     </row>
     <row r="177">
@@ -28028,7 +28028,7 @@
         <v>11.34386655493077</v>
       </c>
       <c r="AB209" t="n">
-        <v>46.50236161075947</v>
+        <v>46.50236161075948</v>
       </c>
     </row>
     <row r="210">
@@ -34364,7 +34364,7 @@
         <v>11.32377083555501</v>
       </c>
       <c r="AB257" t="n">
-        <v>46.48946704070877</v>
+        <v>46.48946704070878</v>
       </c>
     </row>
     <row r="258">
@@ -35420,7 +35420,7 @@
         <v>11.33563412084781</v>
       </c>
       <c r="AB265" t="n">
-        <v>46.4899188529852</v>
+        <v>46.48991885298519</v>
       </c>
     </row>
     <row r="266">
@@ -44528,7 +44528,7 @@
         <v>11.35773610495826</v>
       </c>
       <c r="AB334" t="n">
-        <v>46.49691164116562</v>
+        <v>46.49691164116563</v>
       </c>
     </row>
     <row r="335">
@@ -46772,7 +46772,7 @@
         <v>11.33896586295499</v>
       </c>
       <c r="AB351" t="n">
-        <v>46.48652564654786</v>
+        <v>46.48652564654785</v>
       </c>
     </row>
     <row r="352">
@@ -48752,7 +48752,7 @@
         <v>11.33275239789232</v>
       </c>
       <c r="AB366" t="n">
-        <v>46.4939084170717</v>
+        <v>46.49390841707169</v>
       </c>
     </row>
     <row r="367">
@@ -49280,7 +49280,7 @@
         <v>11.31905779778666</v>
       </c>
       <c r="AB370" t="n">
-        <v>46.48293155588991</v>
+        <v>46.48293155588992</v>
       </c>
     </row>
     <row r="371">
@@ -49808,7 +49808,7 @@
         <v>11.33312829938614</v>
       </c>
       <c r="AB374" t="n">
-        <v>46.47623456188504</v>
+        <v>46.47623456188503</v>
       </c>
     </row>
     <row r="375">
@@ -51128,7 +51128,7 @@
         <v>11.35023041493985</v>
       </c>
       <c r="AB384" t="n">
-        <v>46.51263107455367</v>
+        <v>46.51263107455366</v>
       </c>
     </row>
     <row r="385">
@@ -51260,7 +51260,7 @@
         <v>11.32291194054982</v>
       </c>
       <c r="AB385" t="n">
-        <v>46.49048362365396</v>
+        <v>46.49048362365395</v>
       </c>
     </row>
     <row r="386">
@@ -54296,7 +54296,7 @@
         <v>11.33596968434511</v>
       </c>
       <c r="AB408" t="n">
-        <v>46.49359346096039</v>
+        <v>46.4935934609604</v>
       </c>
     </row>
     <row r="409">
@@ -56804,7 +56804,7 @@
         <v>11.35908748761192</v>
       </c>
       <c r="AB427" t="n">
-        <v>46.49712909790212</v>
+        <v>46.49712909790211</v>
       </c>
     </row>
     <row r="428">
@@ -58124,7 +58124,7 @@
         <v>11.33184348138847</v>
       </c>
       <c r="AB437" t="n">
-        <v>46.49011605386703</v>
+        <v>46.49011605386704</v>
       </c>
     </row>
     <row r="438">
@@ -60632,7 +60632,7 @@
         <v>11.31965974462576</v>
       </c>
       <c r="AB456" t="n">
-        <v>46.49438664158103</v>
+        <v>46.49438664158102</v>
       </c>
     </row>
     <row r="457">

</xml_diff>